<commit_message>
Fixed Dialog box and added method to create New continous database
</commit_message>
<xml_diff>
--- a/Approved Vendors.xlsx
+++ b/Approved Vendors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mckinnin.lloyd\Documents\Projects\Continous Audits\P-card_Personal_Purchases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B512250F-9137-4956-BE7E-AB55CF0AC49D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDED3C3-1ABD-4C2E-839F-A30B87B49E92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11736" windowHeight="5064" xr2:uid="{F944715A-3941-4D36-9860-B89E6E15F66D}"/>
   </bookViews>
@@ -27,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>KOPY KATZ PRINTING</t>
+    <t>Approved Merchant Name</t>
   </si>
   <si>
-    <t>Approved Merchant Name</t>
+    <t>KOPY KATZ PRINTING</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,12 +406,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>